<commit_message>
Changed stair.dwg, AmOfMe.xlsx, unitsPlan.dwg (v1.1)
</commit_message>
<xml_diff>
--- a/Building/AmOfMe.xlsx
+++ b/Building/AmOfMe.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="30">
   <si>
     <t>Марка элемента</t>
   </si>
@@ -99,6 +99,21 @@
   </si>
   <si>
     <t>Закладные 1 этаж</t>
+  </si>
+  <si>
+    <t>1 этаж</t>
+  </si>
+  <si>
+    <t>2 этаж</t>
+  </si>
+  <si>
+    <t>ЗД-19</t>
+  </si>
+  <si>
+    <t>ЗД-20</t>
+  </si>
+  <si>
+    <t>ЗД-21</t>
   </si>
 </sst>
 </file>
@@ -141,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -371,49 +386,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -437,6 +501,58 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,613 +854,1191 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="4" t="s">
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="13"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="N3" s="21"/>
+      <c r="O3" s="23"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="32"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="8">
-        <f>0.4*$B4</f>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3">
+        <f>0.4*$B5</f>
         <v>1.6</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="8">
-        <f>SUM(C4:G4)</f>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="3">
+        <f>SUM(C5:G5)</f>
         <v>1.6</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="8">
-        <f>6.9*$B4</f>
+      <c r="I5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="3">
+        <f>6.9*$B5</f>
         <v>27.6</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" s="8">
-        <f>SUM(I4:L4)</f>
+      <c r="K5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="3">
+        <f>SUM(I5:L5)</f>
         <v>27.6</v>
       </c>
-      <c r="N4" s="8">
-        <f>H4+M4</f>
+      <c r="N5" s="3">
+        <f>H5+M5</f>
         <v>29.200000000000003</v>
       </c>
-      <c r="O4" s="15">
-        <f>N4</f>
+      <c r="O5" s="6">
+        <f>N5</f>
         <v>29.200000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="9">
-        <f>2*$B5</f>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4">
+        <f>2*$B6</f>
         <v>2</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="9">
-        <f t="shared" ref="H5:H10" si="0">SUM(C5:G5)</f>
+      <c r="F6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" ref="H6:H11" si="0">SUM(C6:G6)</f>
         <v>2</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="9">
-        <f>7.5*$B5</f>
+      <c r="I6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="4">
+        <f>7.5*$B6</f>
         <v>7.5</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="9">
-        <f t="shared" ref="M5:M10" si="1">SUM(I5:L5)</f>
+      <c r="K6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="4">
+        <f t="shared" ref="M6:M11" si="1">SUM(I6:L6)</f>
         <v>7.5</v>
       </c>
-      <c r="N5" s="9">
-        <f t="shared" ref="N5:N10" si="2">H5+M5</f>
+      <c r="N6" s="4">
+        <f t="shared" ref="N6:N11" si="2">H6+M6</f>
         <v>9.5</v>
       </c>
-      <c r="O5" s="17">
-        <f t="shared" ref="O5:O10" si="3">N5</f>
+      <c r="O6" s="8">
+        <f t="shared" ref="O6:O11" si="3">N6</f>
         <v>9.5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="9">
-        <f>2.16*$B6</f>
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4">
+        <f>2.16*$B7</f>
         <v>2.16</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="9">
+      <c r="F7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="4">
         <f t="shared" si="0"/>
         <v>2.16</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="9">
-        <f>10.56*$B6</f>
+      <c r="I7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="4">
+        <f>10.56*$B7</f>
         <v>10.56</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="9">
+      <c r="L7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="4">
         <f t="shared" si="1"/>
         <v>10.56</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N7" s="4">
         <f t="shared" si="2"/>
         <v>12.72</v>
       </c>
-      <c r="O6" s="17">
+      <c r="O7" s="8">
         <f t="shared" si="3"/>
         <v>12.72</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B8" s="4">
         <v>18</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="9">
-        <f>2.6*$B7</f>
+      <c r="C8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="4">
+        <f>2.6*$B8</f>
         <v>46.800000000000004</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H8" s="4">
         <f t="shared" si="0"/>
         <v>46.800000000000004</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="9">
-        <f>11.2*$B7</f>
+      <c r="I8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="4">
+        <f>11.2*$B8</f>
         <v>201.6</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M8" s="4">
         <f t="shared" si="1"/>
         <v>201.6</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N8" s="4">
         <f t="shared" si="2"/>
         <v>248.4</v>
       </c>
-      <c r="O7" s="17">
+      <c r="O8" s="8">
         <f t="shared" si="3"/>
         <v>248.4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B9" s="4">
         <v>10</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="9">
-        <f>1.3*$B8</f>
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="4">
+        <f>1.3*$B9</f>
         <v>13</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="9">
+      <c r="G9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="9">
-        <f>5.1*$B8</f>
+      <c r="I9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="4">
+        <f>5.1*$B9</f>
         <v>51</v>
       </c>
-      <c r="L8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="9">
+      <c r="L9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="4">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N9" s="4">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O9" s="8">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B10" s="4">
         <v>189</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="9">
-        <f>1*$B9</f>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="4">
+        <f>1*$B10</f>
         <v>189</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="9">
+      <c r="F10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="4">
         <f t="shared" si="0"/>
         <v>189</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="9">
-        <f>1.4*$B9</f>
+      <c r="I10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="4">
+        <f>1.4*$B10</f>
         <v>264.59999999999997</v>
       </c>
-      <c r="K9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="9">
+      <c r="K10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="4">
         <f t="shared" si="1"/>
         <v>264.59999999999997</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N10" s="4">
         <f t="shared" si="2"/>
         <v>453.59999999999997</v>
       </c>
-      <c r="O9" s="17">
+      <c r="O10" s="8">
         <f t="shared" si="3"/>
         <v>453.59999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B11" s="4">
         <v>19</v>
       </c>
-      <c r="C10" s="9">
-        <f>0.1*$B10</f>
+      <c r="C11" s="4">
+        <f>0.1*$B11</f>
         <v>1.9000000000000001</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="9">
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="4">
         <f t="shared" si="0"/>
         <v>1.9000000000000001</v>
       </c>
-      <c r="I10" s="9">
-        <f>1.4*$B10</f>
+      <c r="I11" s="4">
+        <f>1.4*$B11</f>
         <v>26.599999999999998</v>
       </c>
-      <c r="J10" s="9">
-        <f>0.4*$B10</f>
+      <c r="J11" s="4">
+        <f>0.4*$B11</f>
         <v>7.6000000000000005</v>
       </c>
-      <c r="K10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="9">
+      <c r="K11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="4">
         <f t="shared" si="1"/>
         <v>34.199999999999996</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N11" s="4">
         <f t="shared" si="2"/>
         <v>36.099999999999994</v>
       </c>
-      <c r="O10" s="17">
+      <c r="O11" s="8">
         <f t="shared" si="3"/>
         <v>36.099999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="17"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="8"/>
+    </row>
+    <row r="13" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22">
-        <f>SUM(C4:C11)</f>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25">
+        <f>SUM(C5:C12)</f>
         <v>1.9000000000000001</v>
       </c>
-      <c r="D12" s="22">
-        <f t="shared" ref="D12:O12" si="4">SUM(D4:D11)</f>
+      <c r="D13" s="25">
+        <f>SUM(D5:D12)</f>
         <v>1.6</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E13" s="25">
+        <f>SUM(E5:E12)</f>
+        <v>193.16</v>
+      </c>
+      <c r="F13" s="25">
+        <f>SUM(F5:F12)</f>
+        <v>13</v>
+      </c>
+      <c r="G13" s="25">
+        <f>SUM(G5:G12)</f>
+        <v>46.800000000000004</v>
+      </c>
+      <c r="H13" s="25">
+        <f>SUM(H5:H12)</f>
+        <v>256.45999999999998</v>
+      </c>
+      <c r="I13" s="25">
+        <f>SUM(I5:I12)</f>
+        <v>26.599999999999998</v>
+      </c>
+      <c r="J13" s="25">
+        <f>SUM(J5:J12)</f>
+        <v>307.3</v>
+      </c>
+      <c r="K13" s="25">
+        <f>SUM(K5:K12)</f>
+        <v>61.56</v>
+      </c>
+      <c r="L13" s="25">
+        <f>SUM(L5:L12)</f>
+        <v>201.6</v>
+      </c>
+      <c r="M13" s="25">
+        <f>SUM(M5:M12)</f>
+        <v>597.05999999999995</v>
+      </c>
+      <c r="N13" s="25">
+        <f>SUM(N5:N12)</f>
+        <v>853.52</v>
+      </c>
+      <c r="O13" s="26">
+        <f>SUM(O5:O12)</f>
+        <v>853.52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="29"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="3">
+        <f>0.4*$B15</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="3">
+        <f>SUM(C15:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="3">
+        <f>6.9*$B15</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="3">
+        <f>SUM(I15:L15)</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <f>H15+M15</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="6">
+        <f>N15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="4">
+        <f>2*$B16</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" ref="H16:H21" si="4">SUM(C16:G16)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="4">
+        <f>7.5*$B16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" s="4">
+        <f t="shared" ref="M16:M21" si="5">SUM(I16:L16)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <f t="shared" ref="N16:N21" si="6">H16+M16</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="8">
+        <f t="shared" ref="O16:O21" si="7">N16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="4">
+        <f>2.16*$B17</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="4">
         <f t="shared" si="4"/>
-        <v>193.16</v>
-      </c>
-      <c r="F12" s="22">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="4">
+        <f>10.56*$B17</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="4">
+        <v>6</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="4">
+        <f>2.6*$B18</f>
+        <v>15.600000000000001</v>
+      </c>
+      <c r="H18" s="4">
         <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="G12" s="22">
+        <v>15.600000000000001</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="4">
+        <f>11.2*$B18</f>
+        <v>67.199999999999989</v>
+      </c>
+      <c r="M18" s="4">
+        <f t="shared" si="5"/>
+        <v>67.199999999999989</v>
+      </c>
+      <c r="N18" s="4">
+        <f t="shared" si="6"/>
+        <v>82.799999999999983</v>
+      </c>
+      <c r="O18" s="8">
+        <f t="shared" si="7"/>
+        <v>82.799999999999983</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="4">
+        <v>49</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="4">
+        <f>1.3*$B19</f>
+        <v>63.7</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="4">
         <f t="shared" si="4"/>
-        <v>46.800000000000004</v>
-      </c>
-      <c r="H12" s="22">
+        <v>63.7</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="4">
+        <f>5.1*$B19</f>
+        <v>249.89999999999998</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="4">
+        <f t="shared" si="5"/>
+        <v>249.89999999999998</v>
+      </c>
+      <c r="N19" s="4">
+        <f t="shared" si="6"/>
+        <v>313.59999999999997</v>
+      </c>
+      <c r="O19" s="8">
+        <f t="shared" si="7"/>
+        <v>313.59999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="4">
+        <v>115</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="4">
+        <f>1*$B20</f>
+        <v>115</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="4">
         <f t="shared" si="4"/>
-        <v>256.45999999999998</v>
-      </c>
-      <c r="I12" s="22">
+        <v>115</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="4">
+        <f>1.4*$B20</f>
+        <v>161</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20" s="4">
+        <f t="shared" si="5"/>
+        <v>161</v>
+      </c>
+      <c r="N20" s="4">
+        <f t="shared" si="6"/>
+        <v>276</v>
+      </c>
+      <c r="O20" s="8">
+        <f t="shared" si="7"/>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="4">
+        <v>44</v>
+      </c>
+      <c r="C21" s="4">
+        <f>0.1*$B21</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="4">
         <f t="shared" si="4"/>
-        <v>26.599999999999998</v>
-      </c>
-      <c r="J12" s="22">
-        <f t="shared" si="4"/>
-        <v>307.3</v>
-      </c>
-      <c r="K12" s="22">
-        <f t="shared" si="4"/>
-        <v>61.56</v>
-      </c>
-      <c r="L12" s="22">
-        <f t="shared" si="4"/>
-        <v>201.6</v>
-      </c>
-      <c r="M12" s="22">
-        <f t="shared" si="4"/>
-        <v>597.05999999999995</v>
-      </c>
-      <c r="N12" s="22">
-        <f t="shared" si="4"/>
-        <v>853.52</v>
-      </c>
-      <c r="O12" s="23">
-        <f t="shared" si="4"/>
-        <v>853.52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="17"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="17"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="17"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="17"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="20"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I21" s="4">
+        <f>1.4*$B21</f>
+        <v>61.599999999999994</v>
+      </c>
+      <c r="J21" s="4">
+        <f>0.4*$B21</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="5"/>
+        <v>79.199999999999989</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="6"/>
+        <v>83.6</v>
+      </c>
+      <c r="O21" s="8">
+        <f t="shared" si="7"/>
+        <v>83.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="4">
+        <v>5</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="4">
+        <f>3*$B22</f>
+        <v>15</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" ref="H22" si="8">SUM(C22:G22)</f>
+        <v>15</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" s="4">
+        <f>17.2*$B22</f>
+        <v>86</v>
+      </c>
+      <c r="M22" s="4">
+        <f t="shared" ref="M22" si="9">SUM(I22:L22)</f>
+        <v>86</v>
+      </c>
+      <c r="N22" s="4">
+        <f t="shared" ref="N22" si="10">H22+M22</f>
+        <v>101</v>
+      </c>
+      <c r="O22" s="8">
+        <f t="shared" ref="O22" si="11">N22</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="4">
+        <v>5</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="4">
+        <f>3.7*$B23</f>
+        <v>18.5</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" ref="H23" si="12">SUM(C23:G23)</f>
+        <v>18.5</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L23" s="4">
+        <f>11.4*$B23</f>
+        <v>57</v>
+      </c>
+      <c r="M23" s="4">
+        <f t="shared" ref="M23" si="13">SUM(I23:L23)</f>
+        <v>57</v>
+      </c>
+      <c r="N23" s="4">
+        <f t="shared" ref="N23" si="14">H23+M23</f>
+        <v>75.5</v>
+      </c>
+      <c r="O23" s="8">
+        <f t="shared" ref="O23" si="15">N23</f>
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="4">
+        <v>6</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="4">
+        <f>1.7*$B24</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="4">
+        <f t="shared" ref="H24" si="16">SUM(C24:G24)</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="4">
+        <f>7.5*$B24</f>
+        <v>45</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24" s="4">
+        <f t="shared" ref="M24" si="17">SUM(I24:L24)</f>
+        <v>45</v>
+      </c>
+      <c r="N24" s="4">
+        <f t="shared" ref="N24" si="18">H24+M24</f>
+        <v>55.2</v>
+      </c>
+      <c r="O24" s="8">
+        <f t="shared" ref="O24" si="19">N24</f>
+        <v>55.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="8"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13">
+        <f>SUM(C15:C25)</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D26" s="13">
+        <f>SUM(D15:D25)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="13">
+        <f>SUM(E15:E25)</f>
+        <v>115</v>
+      </c>
+      <c r="F26" s="13">
+        <f>SUM(F15:F25)</f>
+        <v>73.900000000000006</v>
+      </c>
+      <c r="G26" s="13">
+        <f>SUM(G15:G25)</f>
+        <v>49.1</v>
+      </c>
+      <c r="H26" s="13">
+        <f>SUM(H15:H25)</f>
+        <v>242.4</v>
+      </c>
+      <c r="I26" s="13">
+        <f>SUM(I15:I25)</f>
+        <v>61.599999999999994</v>
+      </c>
+      <c r="J26" s="13">
+        <f>SUM(J15:J25)</f>
+        <v>178.6</v>
+      </c>
+      <c r="K26" s="13">
+        <f>SUM(K15:K25)</f>
+        <v>294.89999999999998</v>
+      </c>
+      <c r="L26" s="13">
+        <f>SUM(L15:L25)</f>
+        <v>210.2</v>
+      </c>
+      <c r="M26" s="13">
+        <f>SUM(M15:M25)</f>
+        <v>745.3</v>
+      </c>
+      <c r="N26" s="13">
+        <f>SUM(N15:N25)</f>
+        <v>987.7</v>
+      </c>
+      <c r="O26" s="14">
+        <f>SUM(O15:O25)</f>
+        <v>987.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A14:O14"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Building/, added change 1 in Building/*_c1.dwg
</commit_message>
<xml_diff>
--- a/Building/AmOfMe.xlsx
+++ b/Building/AmOfMe.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25110" windowHeight="10905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25110" windowHeight="10905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист изм1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="0.1"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="102">
   <si>
     <t>Марка элемента</t>
   </si>
@@ -322,6 +323,15 @@
   </si>
   <si>
     <t>пояс 250х150</t>
+  </si>
+  <si>
+    <t>пояс 400х150 тип 1</t>
+  </si>
+  <si>
+    <t>пояс 250х150  тип 3</t>
+  </si>
+  <si>
+    <t>пояс 400х280  тип 2</t>
   </si>
 </sst>
 </file>
@@ -989,6 +999,63 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1006,63 +1073,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1375,43 +1385,43 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="69" t="s">
+      <c r="A2" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="65" t="s">
+      <c r="D2" s="68"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66" t="s">
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="71" t="s">
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="57" t="s">
+      <c r="S2" s="51" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
-      <c r="B3" s="70"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1457,31 +1467,31 @@
       <c r="Q3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="72"/>
-      <c r="S3" s="58"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="52"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="61"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="55"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2029,27 +2039,27 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
-      <c r="L14" s="63"/>
-      <c r="M14" s="63"/>
-      <c r="N14" s="63"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="63"/>
-      <c r="R14" s="63"/>
-      <c r="S14" s="64"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="57"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="58"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -2980,46 +2990,46 @@
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="70" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
       <c r="E36" s="31"/>
-      <c r="F36" s="51" t="s">
+      <c r="F36" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="51" t="s">
+      <c r="G36" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="H36" s="51" t="s">
+      <c r="H36" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="I36" s="51" t="s">
+      <c r="I36" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="J36" s="51">
+      <c r="J36" s="70">
         <v>-8</v>
       </c>
-      <c r="K36" s="53" t="s">
+      <c r="K36" s="72" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
-      <c r="B37" s="52"/>
+      <c r="A37" s="75"/>
+      <c r="B37" s="71"/>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="54"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="73"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
@@ -3231,46 +3241,46 @@
       <c r="A47" s="17"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="55" t="s">
+      <c r="A48" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="51" t="s">
+      <c r="B48" s="70" t="s">
         <v>15</v>
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="31"/>
       <c r="E48" s="31"/>
-      <c r="F48" s="51" t="s">
+      <c r="F48" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="G48" s="51" t="s">
+      <c r="G48" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="H48" s="51" t="s">
+      <c r="H48" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="I48" s="51" t="s">
+      <c r="I48" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="J48" s="51">
+      <c r="J48" s="70">
         <v>-8</v>
       </c>
-      <c r="K48" s="53" t="s">
+      <c r="K48" s="72" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="56"/>
-      <c r="B49" s="52"/>
+      <c r="A49" s="75"/>
+      <c r="B49" s="71"/>
       <c r="C49" s="25"/>
       <c r="D49" s="25"/>
       <c r="E49" s="25"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="52"/>
-      <c r="J49" s="52"/>
-      <c r="K49" s="54"/>
+      <c r="F49" s="71"/>
+      <c r="G49" s="71"/>
+      <c r="H49" s="71"/>
+      <c r="I49" s="71"/>
+      <c r="J49" s="71"/>
+      <c r="K49" s="73"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
@@ -3483,15 +3493,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A14:S14"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:Q2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="C2:E2"/>
     <mergeCell ref="I36:I37"/>
     <mergeCell ref="J36:J37"/>
     <mergeCell ref="K36:K37"/>
@@ -3508,6 +3509,15 @@
     <mergeCell ref="F36:F37"/>
     <mergeCell ref="G36:G37"/>
     <mergeCell ref="H36:H37"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A14:S14"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:Q2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="C2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3518,7 +3528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
@@ -4436,4 +4446,928 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="42"/>
+    <col min="2" max="2" width="31.5703125" style="42" customWidth="1"/>
+    <col min="3" max="10" width="9.140625" style="42"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="20" width="9.140625" style="42"/>
+    <col min="21" max="21" width="28.7109375" style="42" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" style="42" customWidth="1"/>
+    <col min="23" max="23" width="19.28515625" style="42" customWidth="1"/>
+    <col min="24" max="28" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V1" s="76" t="s">
+        <v>80</v>
+      </c>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="78"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="P2" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="R2" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="S2" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="T2" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="U2" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="V2" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="W2" s="43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="G3" s="48">
+        <f>SUM(G4:G10)</f>
+        <v>414.28000000000003</v>
+      </c>
+      <c r="H3" s="44">
+        <f t="shared" ref="H3:N3" si="0">SUM(H4:H10)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="48">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="J3" s="48">
+        <f t="shared" si="0"/>
+        <v>1056.7</v>
+      </c>
+      <c r="K3" s="46">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="L3" s="44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M3" s="44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N3" s="44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44">
+        <f>SUM(P4:P10)</f>
+        <v>106</v>
+      </c>
+      <c r="Q3" s="44">
+        <f>SUM(Q4:Q10)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="44">
+        <v>22</v>
+      </c>
+      <c r="S3" s="44">
+        <f>SUM(S4:S10)</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="44">
+        <f>SUM(T4:T10)</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="48">
+        <f>SUM(U4:U10)</f>
+        <v>4.3499400000000001</v>
+      </c>
+      <c r="W3" s="48">
+        <f>SUM(W4:W19)</f>
+        <v>345.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="42">
+        <v>6.35</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4" s="42">
+        <f>C4*D4</f>
+        <v>31.75</v>
+      </c>
+      <c r="G4" s="42">
+        <f>E4*4</f>
+        <v>127</v>
+      </c>
+      <c r="I4" s="42">
+        <f>D4*4</f>
+        <v>20</v>
+      </c>
+      <c r="J4" s="42">
+        <f>E4*10+D4</f>
+        <v>322.5</v>
+      </c>
+      <c r="K4" s="1">
+        <f>MROUND(E4,5)</f>
+        <v>30</v>
+      </c>
+      <c r="P4" s="42">
+        <f>ROUNDUP(E4,0)</f>
+        <v>32</v>
+      </c>
+      <c r="U4" s="42">
+        <f>E4*0.14*0.3</f>
+        <v>1.3335000000000001</v>
+      </c>
+      <c r="V4" s="42">
+        <v>3</v>
+      </c>
+      <c r="W4" s="42">
+        <f t="shared" ref="W4:W10" si="1">E4*V4</f>
+        <v>95.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="42">
+        <v>4.63</v>
+      </c>
+      <c r="D5" s="42">
+        <v>5</v>
+      </c>
+      <c r="E5" s="42">
+        <f t="shared" ref="E5:E10" si="2">C5*D5</f>
+        <v>23.15</v>
+      </c>
+      <c r="G5" s="42">
+        <f t="shared" ref="G5:G10" si="3">E5*4</f>
+        <v>92.6</v>
+      </c>
+      <c r="I5" s="42">
+        <f>D5*4</f>
+        <v>20</v>
+      </c>
+      <c r="J5" s="42">
+        <f t="shared" ref="J5:J10" si="4">E5*10+D5</f>
+        <v>236.5</v>
+      </c>
+      <c r="P5" s="42">
+        <f t="shared" ref="P5:P10" si="5">ROUNDUP(E5,0)</f>
+        <v>24</v>
+      </c>
+      <c r="U5" s="42">
+        <f t="shared" ref="U5:U10" si="6">E5*0.14*0.3</f>
+        <v>0.97229999999999994</v>
+      </c>
+      <c r="V5" s="42">
+        <v>3</v>
+      </c>
+      <c r="W5" s="42">
+        <f t="shared" si="1"/>
+        <v>69.449999999999989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B6" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="42">
+        <v>8.92</v>
+      </c>
+      <c r="D6" s="42">
+        <v>1</v>
+      </c>
+      <c r="E6" s="42">
+        <f t="shared" si="2"/>
+        <v>8.92</v>
+      </c>
+      <c r="G6" s="42">
+        <f t="shared" si="3"/>
+        <v>35.68</v>
+      </c>
+      <c r="I6" s="42">
+        <f>D6*4</f>
+        <v>4</v>
+      </c>
+      <c r="J6" s="42">
+        <f t="shared" si="4"/>
+        <v>90.2</v>
+      </c>
+      <c r="P6" s="42">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="U6" s="42">
+        <f t="shared" si="6"/>
+        <v>0.37464000000000003</v>
+      </c>
+      <c r="V6" s="42">
+        <v>3</v>
+      </c>
+      <c r="W6" s="42">
+        <f t="shared" si="1"/>
+        <v>26.759999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B7" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="42">
+        <v>7.55</v>
+      </c>
+      <c r="D7" s="42">
+        <v>2</v>
+      </c>
+      <c r="E7" s="42">
+        <f t="shared" si="2"/>
+        <v>15.1</v>
+      </c>
+      <c r="G7" s="42">
+        <f t="shared" si="3"/>
+        <v>60.4</v>
+      </c>
+      <c r="I7" s="42">
+        <f>D7*4</f>
+        <v>8</v>
+      </c>
+      <c r="J7" s="42">
+        <f t="shared" si="4"/>
+        <v>153</v>
+      </c>
+      <c r="P7" s="42">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="U7" s="42">
+        <f t="shared" si="6"/>
+        <v>0.6342000000000001</v>
+      </c>
+      <c r="V7" s="42">
+        <v>3</v>
+      </c>
+      <c r="W7" s="42">
+        <f t="shared" si="1"/>
+        <v>45.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B8" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="42">
+        <v>2.15</v>
+      </c>
+      <c r="D8" s="42">
+        <v>5</v>
+      </c>
+      <c r="E8" s="42">
+        <f t="shared" si="2"/>
+        <v>10.75</v>
+      </c>
+      <c r="G8" s="42">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="I8" s="42">
+        <f>D8*4</f>
+        <v>20</v>
+      </c>
+      <c r="J8" s="42">
+        <f t="shared" si="4"/>
+        <v>112.5</v>
+      </c>
+      <c r="P8" s="42">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="U8" s="42">
+        <f t="shared" si="6"/>
+        <v>0.45150000000000001</v>
+      </c>
+      <c r="V8" s="42">
+        <v>3</v>
+      </c>
+      <c r="W8" s="42">
+        <f t="shared" si="1"/>
+        <v>32.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="42">
+        <v>2.95</v>
+      </c>
+      <c r="D9" s="42">
+        <v>2</v>
+      </c>
+      <c r="E9" s="42">
+        <f t="shared" si="2"/>
+        <v>5.9</v>
+      </c>
+      <c r="G9" s="42">
+        <f t="shared" si="3"/>
+        <v>23.6</v>
+      </c>
+      <c r="I9" s="42">
+        <v>0</v>
+      </c>
+      <c r="J9" s="42">
+        <f t="shared" si="4"/>
+        <v>61</v>
+      </c>
+      <c r="P9" s="42">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="U9" s="42">
+        <f t="shared" si="6"/>
+        <v>0.24780000000000005</v>
+      </c>
+      <c r="V9" s="42">
+        <v>3</v>
+      </c>
+      <c r="W9" s="42">
+        <f t="shared" si="1"/>
+        <v>17.700000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B10" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="42">
+        <v>8</v>
+      </c>
+      <c r="D10" s="42">
+        <v>1</v>
+      </c>
+      <c r="E10" s="42">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G10" s="42">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="I10" s="42">
+        <v>0</v>
+      </c>
+      <c r="J10" s="42">
+        <f t="shared" si="4"/>
+        <v>81</v>
+      </c>
+      <c r="P10" s="42">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="U10" s="42">
+        <f t="shared" si="6"/>
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="V10" s="42">
+        <v>3</v>
+      </c>
+      <c r="W10" s="42">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="48">
+        <f>SUM(G13)</f>
+        <v>62.4</v>
+      </c>
+      <c r="H12" s="44">
+        <f t="shared" ref="H12:N12" si="7">SUM(H13)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="44">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="49">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="46">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="48">
+        <f t="shared" si="7"/>
+        <v>160</v>
+      </c>
+      <c r="M12" s="44">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="44">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44">
+        <f>SUM(P13)</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="44">
+        <f>SUM(Q13)</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="44">
+        <f>SUM(R13)</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="48">
+        <f>SUM(S13)</f>
+        <v>16</v>
+      </c>
+      <c r="T12" s="44">
+        <f>SUM(T13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B13" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="42">
+        <v>3.9</v>
+      </c>
+      <c r="D13" s="42">
+        <v>4</v>
+      </c>
+      <c r="E13" s="42">
+        <f>C13*D13</f>
+        <v>15.6</v>
+      </c>
+      <c r="G13" s="42">
+        <f>E13*4</f>
+        <v>62.4</v>
+      </c>
+      <c r="J13" s="42">
+        <v>0</v>
+      </c>
+      <c r="L13" s="42">
+        <f>E13*10+D13</f>
+        <v>160</v>
+      </c>
+      <c r="S13" s="42">
+        <f>ROUNDUP(E13,0)</f>
+        <v>16</v>
+      </c>
+      <c r="U13" s="42">
+        <f>E13*0.14*0.3</f>
+        <v>0.6552</v>
+      </c>
+      <c r="V13" s="42">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="W13" s="42">
+        <f>E13*V13</f>
+        <v>34.32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="48">
+        <f>SUM(G16:G18)</f>
+        <v>852.8</v>
+      </c>
+      <c r="H15" s="48">
+        <f t="shared" ref="H15:N15" si="8">SUM(H16:H18)</f>
+        <v>375</v>
+      </c>
+      <c r="I15" s="44">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="44">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="46">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="44">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="48">
+        <f t="shared" si="8"/>
+        <v>75</v>
+      </c>
+      <c r="N15" s="48">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="O15" s="48">
+        <v>31</v>
+      </c>
+      <c r="P15" s="44">
+        <f t="shared" ref="P15:U15" si="9">SUM(P16:P18)</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="44">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="44">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="44">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="44">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="48">
+        <f t="shared" si="9"/>
+        <v>12.934799999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B16" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="42">
+        <v>149</v>
+      </c>
+      <c r="E16" s="42">
+        <f>C16</f>
+        <v>149</v>
+      </c>
+      <c r="G16" s="42">
+        <f>E16*4</f>
+        <v>596</v>
+      </c>
+      <c r="H16" s="42">
+        <f>MROUND(E16*2.5, 5)</f>
+        <v>375</v>
+      </c>
+      <c r="U16" s="42">
+        <f>E16*0.4*0.15</f>
+        <v>8.94</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="42">
+        <v>6</v>
+      </c>
+      <c r="E17" s="42">
+        <f>C17</f>
+        <v>6</v>
+      </c>
+      <c r="G17" s="42">
+        <f>E17*4</f>
+        <v>24</v>
+      </c>
+      <c r="N17" s="42">
+        <f>MROUND(E17*2.5,5)</f>
+        <v>15</v>
+      </c>
+      <c r="U17" s="42">
+        <f>E17*0.3*0.15</f>
+        <v>0.26999999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="42">
+        <v>29.1</v>
+      </c>
+      <c r="E18" s="42">
+        <f>C18</f>
+        <v>29.1</v>
+      </c>
+      <c r="G18" s="42">
+        <f>E18*8</f>
+        <v>232.8</v>
+      </c>
+      <c r="M18" s="42">
+        <f>MROUND(E18*2.5,5)</f>
+        <v>75</v>
+      </c>
+      <c r="U18" s="42">
+        <f>E18*0.4*0.32</f>
+        <v>3.7248000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B20" s="43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="50">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="50">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="50">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="50">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="50">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B28" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="42">
+        <v>168</v>
+      </c>
+      <c r="W28" s="48">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B29" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="42">
+        <v>320</v>
+      </c>
+      <c r="W29" s="48">
+        <f>D29*1.5</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E31" s="44">
+        <f>SUM(E32:E35)</f>
+        <v>320.83999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B32" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="42">
+        <v>10.6</v>
+      </c>
+      <c r="D32" s="42">
+        <v>18</v>
+      </c>
+      <c r="E32" s="42">
+        <f>C32*D32</f>
+        <v>190.79999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C33" s="42">
+        <v>7.5</v>
+      </c>
+      <c r="D33" s="42">
+        <v>10</v>
+      </c>
+      <c r="E33" s="42">
+        <f>C33*D33</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C34" s="42">
+        <v>5.76</v>
+      </c>
+      <c r="D34" s="42">
+        <v>4</v>
+      </c>
+      <c r="E34" s="42">
+        <f>C34*D34</f>
+        <v>23.04</v>
+      </c>
+    </row>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C35" s="42">
+        <v>8</v>
+      </c>
+      <c r="D35" s="42">
+        <v>4</v>
+      </c>
+      <c r="E35" s="42">
+        <f>C35*D35</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B37" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="42">
+        <f>SUM(E38:E40)</f>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B38" s="42">
+        <v>400</v>
+      </c>
+      <c r="E38" s="43">
+        <v>499</v>
+      </c>
+      <c r="F38" s="43"/>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B39" s="42">
+        <v>300</v>
+      </c>
+      <c r="E39" s="43">
+        <v>36</v>
+      </c>
+      <c r="F39" s="43"/>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B40" s="42">
+        <v>200</v>
+      </c>
+      <c r="E40" s="43">
+        <f>40+1</f>
+        <v>41</v>
+      </c>
+      <c r="F40" s="43"/>
+    </row>
+    <row r="43" spans="2:23" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B43" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="G43" s="44">
+        <f>SUM(G3,G12,G15)</f>
+        <v>1329.48</v>
+      </c>
+      <c r="H43" s="44">
+        <f t="shared" ref="H43:W43" si="10">SUM(H3,H12,H15)</f>
+        <v>375</v>
+      </c>
+      <c r="I43" s="44">
+        <f t="shared" si="10"/>
+        <v>72</v>
+      </c>
+      <c r="J43" s="44">
+        <f t="shared" si="10"/>
+        <v>1056.7</v>
+      </c>
+      <c r="K43" s="44">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="L43" s="44">
+        <f t="shared" si="10"/>
+        <v>160</v>
+      </c>
+      <c r="M43" s="44">
+        <f t="shared" si="10"/>
+        <v>75</v>
+      </c>
+      <c r="N43" s="44">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="44"/>
+      <c r="S43" s="44"/>
+      <c r="T43" s="44"/>
+      <c r="U43" s="44">
+        <f t="shared" si="10"/>
+        <v>17.284739999999999</v>
+      </c>
+      <c r="V43" s="44">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W43" s="44">
+        <f t="shared" si="10"/>
+        <v>345.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="V1:AA1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added  Building/ *v2, update Fence/Fence.dwg
</commit_message>
<xml_diff>
--- a/Building/AmOfMe.xlsx
+++ b/Building/AmOfMe.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25110" windowHeight="10905" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25110" windowHeight="10905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -999,6 +999,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1055,24 +1073,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1385,43 +1385,43 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="63" t="s">
+      <c r="A2" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="68"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="59" t="s">
+      <c r="D2" s="74"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60" t="s">
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="65" t="s">
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="51" t="s">
+      <c r="S2" s="57" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="64"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1467,31 +1467,31 @@
       <c r="Q3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="66"/>
-      <c r="S3" s="52"/>
+      <c r="R3" s="72"/>
+      <c r="S3" s="58"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="55"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="61"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2039,27 +2039,27 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="58"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="64"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -2990,46 +2990,46 @@
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="74" t="s">
+      <c r="A36" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="70" t="s">
+      <c r="B36" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
       <c r="E36" s="31"/>
-      <c r="F36" s="70" t="s">
+      <c r="F36" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="70" t="s">
+      <c r="G36" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="H36" s="70" t="s">
+      <c r="H36" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="I36" s="70" t="s">
+      <c r="I36" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="J36" s="70">
+      <c r="J36" s="51">
         <v>-8</v>
       </c>
-      <c r="K36" s="72" t="s">
+      <c r="K36" s="53" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="75"/>
-      <c r="B37" s="71"/>
+      <c r="A37" s="56"/>
+      <c r="B37" s="52"/>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
-      <c r="F37" s="71"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="71"/>
-      <c r="J37" s="71"/>
-      <c r="K37" s="73"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="54"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
@@ -3241,46 +3241,46 @@
       <c r="A47" s="17"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="74" t="s">
+      <c r="A48" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="70" t="s">
+      <c r="B48" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="31"/>
       <c r="E48" s="31"/>
-      <c r="F48" s="70" t="s">
+      <c r="F48" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="G48" s="70" t="s">
+      <c r="G48" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="H48" s="70" t="s">
+      <c r="H48" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="I48" s="70" t="s">
+      <c r="I48" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="J48" s="70">
+      <c r="J48" s="51">
         <v>-8</v>
       </c>
-      <c r="K48" s="72" t="s">
+      <c r="K48" s="53" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="75"/>
-      <c r="B49" s="71"/>
+      <c r="A49" s="56"/>
+      <c r="B49" s="52"/>
       <c r="C49" s="25"/>
       <c r="D49" s="25"/>
       <c r="E49" s="25"/>
-      <c r="F49" s="71"/>
-      <c r="G49" s="71"/>
-      <c r="H49" s="71"/>
-      <c r="I49" s="71"/>
-      <c r="J49" s="71"/>
-      <c r="K49" s="73"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="54"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
@@ -3493,6 +3493,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A14:S14"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:Q2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="C2:E2"/>
     <mergeCell ref="I36:I37"/>
     <mergeCell ref="J36:J37"/>
     <mergeCell ref="K36:K37"/>
@@ -3509,15 +3518,6 @@
     <mergeCell ref="F36:F37"/>
     <mergeCell ref="G36:G37"/>
     <mergeCell ref="H36:H37"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A14:S14"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:Q2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="C2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4453,7 +4453,7 @@
   <dimension ref="A1:AB43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5040,7 +5040,7 @@
       </c>
       <c r="M15" s="48">
         <f t="shared" si="8"/>
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="N15" s="48">
         <f t="shared" si="8"/>
@@ -5138,8 +5138,8 @@
         <v>232.8</v>
       </c>
       <c r="M18" s="42">
-        <f>MROUND(E18*2.5,5)</f>
-        <v>75</v>
+        <f>MROUND(E18*5,5)</f>
+        <v>145</v>
       </c>
       <c r="U18" s="42">
         <f>E18*0.4*0.32</f>
@@ -5338,7 +5338,7 @@
       </c>
       <c r="M43" s="44">
         <f t="shared" si="10"/>
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="N43" s="44">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
finish version for building (manufactory)
</commit_message>
<xml_diff>
--- a/Building/AmOfMe.xlsx
+++ b/Building/AmOfMe.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25110" windowHeight="10905" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25110" windowHeight="10905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -338,7 +338,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +434,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -443,7 +451,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -857,11 +865,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -999,6 +1022,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1081,6 +1110,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1385,43 +1450,43 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="69" t="s">
+      <c r="A2" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="65" t="s">
+      <c r="D2" s="76"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66" t="s">
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="71" t="s">
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="57" t="s">
+      <c r="S2" s="59" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
-      <c r="B3" s="70"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1467,31 +1532,31 @@
       <c r="Q3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="72"/>
-      <c r="S3" s="58"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="60"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="61"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="63"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2039,27 +2104,27 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
-      <c r="L14" s="63"/>
-      <c r="M14" s="63"/>
-      <c r="N14" s="63"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="63"/>
-      <c r="R14" s="63"/>
-      <c r="S14" s="64"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="65"/>
+      <c r="S14" s="66"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -2990,46 +3055,46 @@
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
       <c r="E36" s="31"/>
-      <c r="F36" s="51" t="s">
+      <c r="F36" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="51" t="s">
+      <c r="G36" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="H36" s="51" t="s">
+      <c r="H36" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="I36" s="51" t="s">
+      <c r="I36" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="J36" s="51">
+      <c r="J36" s="53">
         <v>-8</v>
       </c>
-      <c r="K36" s="53" t="s">
+      <c r="K36" s="55" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
-      <c r="B37" s="52"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="54"/>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="54"/>
+      <c r="K37" s="56"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
@@ -3241,46 +3306,46 @@
       <c r="A47" s="17"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="55" t="s">
+      <c r="A48" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="51" t="s">
+      <c r="B48" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="31"/>
       <c r="E48" s="31"/>
-      <c r="F48" s="51" t="s">
+      <c r="F48" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="G48" s="51" t="s">
+      <c r="G48" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="H48" s="51" t="s">
+      <c r="H48" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="I48" s="51" t="s">
+      <c r="I48" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="J48" s="51">
+      <c r="J48" s="53">
         <v>-8</v>
       </c>
-      <c r="K48" s="53" t="s">
+      <c r="K48" s="55" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="56"/>
-      <c r="B49" s="52"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="54"/>
       <c r="C49" s="25"/>
       <c r="D49" s="25"/>
       <c r="E49" s="25"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="52"/>
-      <c r="J49" s="52"/>
-      <c r="K49" s="54"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="54"/>
+      <c r="J49" s="54"/>
+      <c r="K49" s="56"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
@@ -3546,14 +3611,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="V1" s="76" t="s">
+      <c r="V1" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="78"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="80"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" s="43"/>
@@ -4452,8 +4517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4469,899 +4534,1832 @@
     <col min="24" max="28" width="9.140625" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="V1" s="76" t="s">
+    <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="81"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="78"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="43"/>
-      <c r="C2" s="43" t="s">
+      <c r="W1" s="82"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
+      <c r="Z1" s="82"/>
+      <c r="AA1" s="82"/>
+    </row>
+    <row r="2" spans="1:27" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43" t="s">
+      <c r="F2" s="85"/>
+      <c r="G2" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="J2" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="45" t="s">
+      <c r="K2" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="L2" s="43" t="s">
+      <c r="L2" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="85" t="s">
         <v>87</v>
       </c>
-      <c r="N2" s="43" t="s">
+      <c r="N2" s="85" t="s">
         <v>88</v>
       </c>
-      <c r="O2" s="43" t="s">
+      <c r="O2" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="P2" s="43" t="s">
+      <c r="P2" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="Q2" s="43" t="s">
+      <c r="Q2" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="R2" s="43" t="s">
+      <c r="R2" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="S2" s="43" t="s">
+      <c r="S2" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="T2" s="43" t="s">
+      <c r="T2" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="U2" s="43" t="s">
+      <c r="U2" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="V2" s="43" t="s">
+      <c r="V2" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="W2" s="43" t="s">
+      <c r="W2" s="85" t="s">
         <v>75</v>
       </c>
+      <c r="X2" s="92"/>
+      <c r="Y2" s="92"/>
+      <c r="Z2" s="92"/>
+      <c r="AA2" s="92"/>
     </row>
     <row r="3" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="43" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="G3" s="48">
+      <c r="C3" s="83"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="84">
         <f>SUM(G4:G10)</f>
         <v>414.28000000000003</v>
       </c>
-      <c r="H3" s="44">
+      <c r="H3" s="85">
         <f t="shared" ref="H3:N3" si="0">SUM(H4:H10)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="48">
+      <c r="I3" s="84">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="J3" s="48">
+      <c r="J3" s="84">
         <f t="shared" si="0"/>
         <v>1056.7</v>
       </c>
-      <c r="K3" s="46">
+      <c r="K3" s="86">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="L3" s="44">
+      <c r="L3" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M3" s="44">
+      <c r="M3" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N3" s="44">
+      <c r="N3" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44">
+      <c r="O3" s="85"/>
+      <c r="P3" s="85">
         <f>SUM(P4:P10)</f>
         <v>106</v>
       </c>
-      <c r="Q3" s="44">
+      <c r="Q3" s="85">
         <f>SUM(Q4:Q10)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="44">
-        <v>22</v>
-      </c>
-      <c r="S3" s="44">
+      <c r="R3" s="85">
+        <v>22</v>
+      </c>
+      <c r="S3" s="85">
         <f>SUM(S4:S10)</f>
         <v>0</v>
       </c>
-      <c r="T3" s="44">
+      <c r="T3" s="85">
         <f>SUM(T4:T10)</f>
         <v>0</v>
       </c>
-      <c r="U3" s="48">
+      <c r="U3" s="84">
         <f>SUM(U4:U10)</f>
         <v>4.3499400000000001</v>
       </c>
-      <c r="W3" s="48">
+      <c r="V3" s="26"/>
+      <c r="W3" s="84">
         <f>SUM(W4:W19)</f>
         <v>345.03</v>
       </c>
+      <c r="X3" s="26"/>
+      <c r="Y3" s="26"/>
+      <c r="Z3" s="26"/>
+      <c r="AA3" s="26"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="26">
         <v>6.35</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="52">
         <v>5</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="26">
         <f>C4*D4</f>
         <v>31.75</v>
       </c>
-      <c r="G4" s="42">
+      <c r="F4" s="26"/>
+      <c r="G4" s="26">
         <f>E4*4</f>
         <v>127</v>
       </c>
-      <c r="I4" s="42">
+      <c r="H4" s="26"/>
+      <c r="I4" s="26">
         <f>D4*4</f>
         <v>20</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="26">
         <f>E4*10+D4</f>
         <v>322.5</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="52">
         <f>MROUND(E4,5)</f>
         <v>30</v>
       </c>
-      <c r="P4" s="42">
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26">
         <f>ROUNDUP(E4,0)</f>
         <v>32</v>
       </c>
-      <c r="U4" s="42">
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26">
         <f>E4*0.14*0.3</f>
         <v>1.3335000000000001</v>
       </c>
-      <c r="V4" s="42">
+      <c r="V4" s="26">
         <v>3</v>
       </c>
-      <c r="W4" s="42">
+      <c r="W4" s="26">
         <f t="shared" ref="W4:W10" si="1">E4*V4</f>
         <v>95.25</v>
       </c>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="26">
         <v>4.63</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="26">
         <v>5</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="26">
         <f t="shared" ref="E5:E10" si="2">C5*D5</f>
         <v>23.15</v>
       </c>
-      <c r="G5" s="42">
+      <c r="F5" s="26"/>
+      <c r="G5" s="26">
         <f t="shared" ref="G5:G10" si="3">E5*4</f>
         <v>92.6</v>
       </c>
-      <c r="I5" s="42">
+      <c r="H5" s="26"/>
+      <c r="I5" s="26">
         <f>D5*4</f>
         <v>20</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="26">
         <f t="shared" ref="J5:J10" si="4">E5*10+D5</f>
         <v>236.5</v>
       </c>
-      <c r="P5" s="42">
+      <c r="K5" s="52"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26">
         <f t="shared" ref="P5:P10" si="5">ROUNDUP(E5,0)</f>
         <v>24</v>
       </c>
-      <c r="U5" s="42">
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26">
         <f t="shared" ref="U5:U10" si="6">E5*0.14*0.3</f>
         <v>0.97229999999999994</v>
       </c>
-      <c r="V5" s="42">
+      <c r="V5" s="26">
         <v>3</v>
       </c>
-      <c r="W5" s="42">
+      <c r="W5" s="26">
         <f t="shared" si="1"/>
         <v>69.449999999999989</v>
       </c>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="26">
         <v>8.92</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="26">
         <v>1</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="26">
         <f t="shared" si="2"/>
         <v>8.92</v>
       </c>
-      <c r="G6" s="42">
+      <c r="F6" s="26"/>
+      <c r="G6" s="26">
         <f t="shared" si="3"/>
         <v>35.68</v>
       </c>
-      <c r="I6" s="42">
+      <c r="H6" s="26"/>
+      <c r="I6" s="26">
         <f>D6*4</f>
         <v>4</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="26">
         <f t="shared" si="4"/>
         <v>90.2</v>
       </c>
-      <c r="P6" s="42">
+      <c r="K6" s="52"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="U6" s="42">
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26">
         <f t="shared" si="6"/>
         <v>0.37464000000000003</v>
       </c>
-      <c r="V6" s="42">
+      <c r="V6" s="26">
         <v>3</v>
       </c>
-      <c r="W6" s="42">
+      <c r="W6" s="26">
         <f t="shared" si="1"/>
         <v>26.759999999999998</v>
       </c>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="26">
         <v>7.55</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="26">
         <v>2</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="26">
         <f t="shared" si="2"/>
         <v>15.1</v>
       </c>
-      <c r="G7" s="42">
+      <c r="F7" s="26"/>
+      <c r="G7" s="26">
         <f t="shared" si="3"/>
         <v>60.4</v>
       </c>
-      <c r="I7" s="42">
+      <c r="H7" s="26"/>
+      <c r="I7" s="26">
         <f>D7*4</f>
         <v>8</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="26">
         <f t="shared" si="4"/>
         <v>153</v>
       </c>
-      <c r="P7" s="42">
+      <c r="K7" s="52"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="U7" s="42">
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26">
         <f t="shared" si="6"/>
         <v>0.6342000000000001</v>
       </c>
-      <c r="V7" s="42">
+      <c r="V7" s="26">
         <v>3</v>
       </c>
-      <c r="W7" s="42">
+      <c r="W7" s="26">
         <f t="shared" si="1"/>
         <v>45.3</v>
       </c>
+      <c r="X7" s="26"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
+      <c r="AA7" s="26"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="42" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="26">
         <v>2.15</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="26">
         <v>5</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="26">
         <f t="shared" si="2"/>
         <v>10.75</v>
       </c>
-      <c r="G8" s="42">
+      <c r="F8" s="26"/>
+      <c r="G8" s="26">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="I8" s="42">
+      <c r="H8" s="26"/>
+      <c r="I8" s="26">
         <f>D8*4</f>
         <v>20</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="26">
         <f t="shared" si="4"/>
         <v>112.5</v>
       </c>
-      <c r="P8" s="42">
+      <c r="K8" s="52"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="U8" s="42">
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="26">
         <f t="shared" si="6"/>
         <v>0.45150000000000001</v>
       </c>
-      <c r="V8" s="42">
+      <c r="V8" s="26">
         <v>3</v>
       </c>
-      <c r="W8" s="42">
+      <c r="W8" s="26">
         <f t="shared" si="1"/>
         <v>32.25</v>
       </c>
+      <c r="X8" s="26"/>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="26"/>
+      <c r="AA8" s="26"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="26">
         <v>2.95</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="26">
         <v>2</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="26">
         <f t="shared" si="2"/>
         <v>5.9</v>
       </c>
-      <c r="G9" s="42">
+      <c r="F9" s="26"/>
+      <c r="G9" s="26">
         <f t="shared" si="3"/>
         <v>23.6</v>
       </c>
-      <c r="I9" s="42">
-        <v>0</v>
-      </c>
-      <c r="J9" s="42">
+      <c r="H9" s="26"/>
+      <c r="I9" s="26">
+        <v>0</v>
+      </c>
+      <c r="J9" s="26">
         <f t="shared" si="4"/>
         <v>61</v>
       </c>
-      <c r="P9" s="42">
+      <c r="K9" s="52"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="U9" s="42">
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="26">
         <f t="shared" si="6"/>
         <v>0.24780000000000005</v>
       </c>
-      <c r="V9" s="42">
+      <c r="V9" s="26">
         <v>3</v>
       </c>
-      <c r="W9" s="42">
+      <c r="W9" s="26">
         <f t="shared" si="1"/>
         <v>17.700000000000003</v>
       </c>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="26"/>
+      <c r="AA9" s="26"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="26">
         <v>8</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="26">
         <v>1</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="26">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="G10" s="42">
+      <c r="F10" s="26"/>
+      <c r="G10" s="26">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="I10" s="42">
-        <v>0</v>
-      </c>
-      <c r="J10" s="42">
+      <c r="H10" s="26"/>
+      <c r="I10" s="26">
+        <v>0</v>
+      </c>
+      <c r="J10" s="26">
         <f t="shared" si="4"/>
         <v>81</v>
       </c>
-      <c r="P10" s="42">
+      <c r="K10" s="52"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="U10" s="42">
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26">
         <f t="shared" si="6"/>
         <v>0.33600000000000002</v>
       </c>
-      <c r="V10" s="42">
+      <c r="V10" s="26">
         <v>3</v>
       </c>
-      <c r="W10" s="42">
+      <c r="W10" s="26">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="26"/>
+      <c r="AA10" s="26"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="26"/>
     </row>
     <row r="12" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="43" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="48">
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="84">
         <f>SUM(G13)</f>
         <v>62.4</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="85">
         <f t="shared" ref="H12:N12" si="7">SUM(H13)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="44">
+      <c r="I12" s="85">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J12" s="49">
+      <c r="J12" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K12" s="46">
+      <c r="K12" s="86">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="L12" s="48">
+      <c r="L12" s="84">
         <f t="shared" si="7"/>
         <v>160</v>
       </c>
-      <c r="M12" s="44">
+      <c r="M12" s="85">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N12" s="44">
+      <c r="N12" s="85">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44">
+      <c r="O12" s="85"/>
+      <c r="P12" s="85">
         <f>SUM(P13)</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="44">
+      <c r="Q12" s="85">
         <f>SUM(Q13)</f>
         <v>0</v>
       </c>
-      <c r="R12" s="44">
+      <c r="R12" s="85">
         <f>SUM(R13)</f>
         <v>0</v>
       </c>
-      <c r="S12" s="48">
+      <c r="S12" s="84">
         <f>SUM(S13)</f>
         <v>16</v>
       </c>
-      <c r="T12" s="44">
+      <c r="T12" s="85">
         <f>SUM(T13)</f>
         <v>0</v>
       </c>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B13" s="42" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="26">
         <v>3.9</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="26">
         <v>4</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="26">
         <f>C13*D13</f>
         <v>15.6</v>
       </c>
-      <c r="G13" s="42">
+      <c r="F13" s="26"/>
+      <c r="G13" s="26">
         <f>E13*4</f>
         <v>62.4</v>
       </c>
-      <c r="J13" s="42">
-        <v>0</v>
-      </c>
-      <c r="L13" s="42">
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26">
+        <v>0</v>
+      </c>
+      <c r="K13" s="52"/>
+      <c r="L13" s="26">
         <f>E13*10+D13</f>
         <v>160</v>
       </c>
-      <c r="S13" s="42">
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26">
         <f>ROUNDUP(E13,0)</f>
         <v>16</v>
       </c>
-      <c r="U13" s="42">
+      <c r="T13" s="26"/>
+      <c r="U13" s="26">
         <f>E13*0.14*0.3</f>
         <v>0.6552</v>
       </c>
-      <c r="V13" s="42">
+      <c r="V13" s="26">
         <v>2.2000000000000002</v>
       </c>
-      <c r="W13" s="42">
+      <c r="W13" s="26">
         <f>E13*V13</f>
         <v>34.32</v>
       </c>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="26"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="26"/>
     </row>
     <row r="15" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="43" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="48">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="84">
         <f>SUM(G16:G18)</f>
         <v>852.8</v>
       </c>
-      <c r="H15" s="48">
+      <c r="H15" s="84">
         <f t="shared" ref="H15:N15" si="8">SUM(H16:H18)</f>
         <v>375</v>
       </c>
-      <c r="I15" s="44">
+      <c r="I15" s="85">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J15" s="44">
+      <c r="J15" s="85">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K15" s="46">
+      <c r="K15" s="86">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L15" s="44">
+      <c r="L15" s="85">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="M15" s="48">
+      <c r="M15" s="84">
         <f t="shared" si="8"/>
         <v>145</v>
       </c>
-      <c r="N15" s="48">
+      <c r="N15" s="84">
         <f t="shared" si="8"/>
         <v>15</v>
       </c>
-      <c r="O15" s="48">
+      <c r="O15" s="84">
         <v>31</v>
       </c>
-      <c r="P15" s="44">
+      <c r="P15" s="85">
         <f t="shared" ref="P15:U15" si="9">SUM(P16:P18)</f>
         <v>0</v>
       </c>
-      <c r="Q15" s="44">
+      <c r="Q15" s="85">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R15" s="44">
+      <c r="R15" s="85">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="S15" s="44">
+      <c r="S15" s="85">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="T15" s="44">
+      <c r="T15" s="85">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U15" s="48">
+      <c r="U15" s="84">
         <f t="shared" si="9"/>
         <v>12.934799999999999</v>
       </c>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B16" s="42" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="42">
+      <c r="C16" s="26">
         <v>149</v>
       </c>
-      <c r="E16" s="42">
+      <c r="D16" s="26"/>
+      <c r="E16" s="26">
         <f>C16</f>
         <v>149</v>
       </c>
-      <c r="G16" s="42">
+      <c r="F16" s="26"/>
+      <c r="G16" s="26">
         <f>E16*4</f>
         <v>596</v>
       </c>
-      <c r="H16" s="42">
+      <c r="H16" s="26">
         <f>MROUND(E16*2.5, 5)</f>
         <v>375</v>
       </c>
-      <c r="U16" s="42">
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="26">
         <f>E16*0.4*0.15</f>
         <v>8.94</v>
       </c>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="s">
+      <c r="V16" s="26"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="26"/>
+      <c r="Y16" s="26"/>
+      <c r="Z16" s="26"/>
+      <c r="AA16" s="26"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="26">
         <v>6</v>
       </c>
-      <c r="E17" s="42">
+      <c r="D17" s="26"/>
+      <c r="E17" s="26">
         <f>C17</f>
         <v>6</v>
       </c>
-      <c r="G17" s="42">
+      <c r="F17" s="26"/>
+      <c r="G17" s="26">
         <f>E17*4</f>
         <v>24</v>
       </c>
-      <c r="N17" s="42">
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26">
         <f>MROUND(E17*2.5,5)</f>
         <v>15</v>
       </c>
-      <c r="U17" s="42">
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="26"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="26">
         <f>E17*0.3*0.15</f>
         <v>0.26999999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="42" t="s">
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="26"/>
+      <c r="AA17" s="26"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="26">
         <v>29.1</v>
       </c>
-      <c r="E18" s="42">
+      <c r="D18" s="26"/>
+      <c r="E18" s="26">
         <f>C18</f>
         <v>29.1</v>
       </c>
-      <c r="G18" s="42">
+      <c r="F18" s="26"/>
+      <c r="G18" s="26">
         <f>E18*8</f>
         <v>232.8</v>
       </c>
-      <c r="M18" s="42">
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26">
         <f>MROUND(E18*5,5)</f>
         <v>145</v>
       </c>
-      <c r="U18" s="42">
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="26"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="26">
         <f>E18*0.4*0.32</f>
         <v>3.7248000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="V18" s="26"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="26"/>
+      <c r="Y18" s="26"/>
+      <c r="Z18" s="26"/>
+      <c r="AA18" s="26"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="26"/>
+      <c r="Z19" s="26"/>
+      <c r="AA19" s="26"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="83" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="42" t="s">
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="26"/>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="26"/>
+      <c r="AA20" s="26"/>
+    </row>
+    <row r="21" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="50">
+      <c r="C21" s="26"/>
+      <c r="D21" s="88">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="42" t="s">
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="26"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="26"/>
+      <c r="Y21" s="26"/>
+      <c r="Z21" s="26"/>
+      <c r="AA21" s="26"/>
+    </row>
+    <row r="22" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="50">
+      <c r="C22" s="26"/>
+      <c r="D22" s="88">
         <v>145</v>
       </c>
-    </row>
-    <row r="23" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="42" t="s">
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
+      <c r="Y22" s="26"/>
+      <c r="Z22" s="26"/>
+      <c r="AA22" s="26"/>
+    </row>
+    <row r="23" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="50">
+      <c r="C23" s="26"/>
+      <c r="D23" s="88">
         <v>255</v>
       </c>
-    </row>
-    <row r="24" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="42" t="s">
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="26"/>
+      <c r="Z23" s="26"/>
+      <c r="AA23" s="26"/>
+    </row>
+    <row r="24" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="50">
+      <c r="C24" s="26"/>
+      <c r="D24" s="88">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="42" t="s">
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
+      <c r="Y24" s="26"/>
+      <c r="Z24" s="26"/>
+      <c r="AA24" s="26"/>
+    </row>
+    <row r="25" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+      <c r="B25" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="50">
+      <c r="C25" s="26"/>
+      <c r="D25" s="88">
         <v>160</v>
       </c>
-    </row>
-    <row r="28" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B28" s="42" t="s">
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="26"/>
+      <c r="V25" s="26"/>
+      <c r="W25" s="26"/>
+      <c r="X25" s="26"/>
+      <c r="Y25" s="26"/>
+      <c r="Z25" s="26"/>
+      <c r="AA25" s="26"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
+      <c r="AA26" s="26"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="26"/>
+      <c r="S27" s="26"/>
+      <c r="T27" s="26"/>
+      <c r="U27" s="26"/>
+      <c r="V27" s="26"/>
+      <c r="W27" s="26"/>
+      <c r="X27" s="26"/>
+      <c r="Y27" s="26"/>
+      <c r="Z27" s="26"/>
+      <c r="AA27" s="26"/>
+    </row>
+    <row r="28" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="42">
+      <c r="C28" s="26"/>
+      <c r="D28" s="26">
         <v>168</v>
       </c>
-      <c r="W28" s="48">
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="26"/>
+      <c r="V28" s="26"/>
+      <c r="W28" s="84">
         <v>700</v>
       </c>
-    </row>
-    <row r="29" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B29" s="42" t="s">
+      <c r="X28" s="26"/>
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="26"/>
+      <c r="AA28" s="26"/>
+    </row>
+    <row r="29" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="42">
+      <c r="C29" s="26"/>
+      <c r="D29" s="26">
         <v>320</v>
       </c>
-      <c r="W29" s="48">
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="84">
         <f>D29*1.5</f>
         <v>480</v>
       </c>
-    </row>
-    <row r="31" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E31" s="44">
+      <c r="X29" s="26"/>
+      <c r="Y29" s="26"/>
+      <c r="Z29" s="26"/>
+      <c r="AA29" s="26"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="26"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="26"/>
+      <c r="X30" s="26"/>
+      <c r="Y30" s="26"/>
+      <c r="Z30" s="26"/>
+      <c r="AA30" s="26"/>
+    </row>
+    <row r="31" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="85">
         <f>SUM(E32:E35)</f>
         <v>320.83999999999997</v>
       </c>
-    </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B32" s="42" t="s">
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="26"/>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="26"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="26"/>
+      <c r="U31" s="26"/>
+      <c r="V31" s="26"/>
+      <c r="W31" s="26"/>
+      <c r="X31" s="26"/>
+      <c r="Y31" s="26"/>
+      <c r="Z31" s="26"/>
+      <c r="AA31" s="26"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
+      <c r="B32" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="42">
+      <c r="C32" s="26">
         <v>10.6</v>
       </c>
-      <c r="D32" s="42">
+      <c r="D32" s="26">
         <v>18</v>
       </c>
-      <c r="E32" s="42">
+      <c r="E32" s="26">
         <f>C32*D32</f>
         <v>190.79999999999998</v>
       </c>
-    </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C33" s="42">
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="26"/>
+      <c r="V32" s="26"/>
+      <c r="W32" s="26"/>
+      <c r="X32" s="26"/>
+      <c r="Y32" s="26"/>
+      <c r="Z32" s="26"/>
+      <c r="AA32" s="26"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26">
         <v>7.5</v>
       </c>
-      <c r="D33" s="42">
+      <c r="D33" s="26">
         <v>10</v>
       </c>
-      <c r="E33" s="42">
+      <c r="E33" s="26">
         <f>C33*D33</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C34" s="42">
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="26"/>
+      <c r="X33" s="26"/>
+      <c r="Y33" s="26"/>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="26"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26">
         <v>5.76</v>
       </c>
-      <c r="D34" s="42">
+      <c r="D34" s="26">
         <v>4</v>
       </c>
-      <c r="E34" s="42">
+      <c r="E34" s="26">
         <f>C34*D34</f>
         <v>23.04</v>
       </c>
-    </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C35" s="42">
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="26"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="26"/>
+      <c r="T34" s="26"/>
+      <c r="U34" s="26"/>
+      <c r="V34" s="26"/>
+      <c r="W34" s="26"/>
+      <c r="X34" s="26"/>
+      <c r="Y34" s="26"/>
+      <c r="Z34" s="26"/>
+      <c r="AA34" s="26"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26">
         <v>8</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D35" s="26">
         <v>4</v>
       </c>
-      <c r="E35" s="42">
+      <c r="E35" s="26">
         <f>C35*D35</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B37" s="42" t="s">
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="26"/>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26"/>
+      <c r="Q35" s="26"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="26"/>
+      <c r="T35" s="26"/>
+      <c r="U35" s="26"/>
+      <c r="V35" s="26"/>
+      <c r="W35" s="26"/>
+      <c r="X35" s="26"/>
+      <c r="Y35" s="26"/>
+      <c r="Z35" s="26"/>
+      <c r="AA35" s="26"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="26"/>
+      <c r="Q36" s="26"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="26"/>
+      <c r="T36" s="26"/>
+      <c r="U36" s="26"/>
+      <c r="V36" s="26"/>
+      <c r="W36" s="26"/>
+      <c r="X36" s="26"/>
+      <c r="Y36" s="26"/>
+      <c r="Z36" s="26"/>
+      <c r="AA36" s="26"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="E37" s="42">
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26">
         <f>SUM(E38:E40)</f>
         <v>576</v>
       </c>
-    </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B38" s="42">
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="26"/>
+      <c r="V37" s="26"/>
+      <c r="W37" s="26"/>
+      <c r="X37" s="26"/>
+      <c r="Y37" s="26"/>
+      <c r="Z37" s="26"/>
+      <c r="AA37" s="26"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A38" s="26"/>
+      <c r="B38" s="26">
         <v>400</v>
       </c>
-      <c r="E38" s="43">
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="83">
         <v>499</v>
       </c>
-      <c r="F38" s="43"/>
-    </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B39" s="42">
+      <c r="F38" s="83"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="52"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="26"/>
+      <c r="W38" s="26"/>
+      <c r="X38" s="26"/>
+      <c r="Y38" s="26"/>
+      <c r="Z38" s="26"/>
+      <c r="AA38" s="26"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
+      <c r="B39" s="26">
         <v>300</v>
       </c>
-      <c r="E39" s="43">
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="83">
         <v>36</v>
       </c>
-      <c r="F39" s="43"/>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B40" s="42">
+      <c r="F39" s="83"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
+      <c r="P39" s="26"/>
+      <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="26"/>
+      <c r="W39" s="26"/>
+      <c r="X39" s="26"/>
+      <c r="Y39" s="26"/>
+      <c r="Z39" s="26"/>
+      <c r="AA39" s="26"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A40" s="26"/>
+      <c r="B40" s="26">
         <v>200</v>
       </c>
-      <c r="E40" s="43">
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="83">
         <f>40+1</f>
         <v>41</v>
       </c>
-      <c r="F40" s="43"/>
-    </row>
-    <row r="43" spans="2:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B43" s="47" t="s">
+      <c r="F40" s="83"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26"/>
+      <c r="S40" s="26"/>
+      <c r="T40" s="26"/>
+      <c r="U40" s="26"/>
+      <c r="V40" s="26"/>
+      <c r="W40" s="26"/>
+      <c r="X40" s="26"/>
+      <c r="Y40" s="26"/>
+      <c r="Z40" s="26"/>
+      <c r="AA40" s="26"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="52"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="26"/>
+      <c r="T41" s="26"/>
+      <c r="U41" s="26"/>
+      <c r="V41" s="26"/>
+      <c r="W41" s="26"/>
+      <c r="X41" s="26"/>
+      <c r="Y41" s="26"/>
+      <c r="Z41" s="26"/>
+      <c r="AA41" s="26"/>
+    </row>
+    <row r="42" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="28"/>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="28"/>
+      <c r="V42" s="28"/>
+      <c r="W42" s="28"/>
+      <c r="X42" s="28"/>
+      <c r="Y42" s="28"/>
+      <c r="Z42" s="28"/>
+      <c r="AA42" s="28"/>
+    </row>
+    <row r="43" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="89"/>
+      <c r="B43" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="G43" s="44">
+      <c r="C43" s="89"/>
+      <c r="D43" s="89"/>
+      <c r="E43" s="89"/>
+      <c r="F43" s="89"/>
+      <c r="G43" s="91">
         <f>SUM(G3,G12,G15)</f>
         <v>1329.48</v>
       </c>
-      <c r="H43" s="44">
+      <c r="H43" s="91">
         <f t="shared" ref="H43:W43" si="10">SUM(H3,H12,H15)</f>
         <v>375</v>
       </c>
-      <c r="I43" s="44">
+      <c r="I43" s="91">
         <f t="shared" si="10"/>
         <v>72</v>
       </c>
-      <c r="J43" s="44">
+      <c r="J43" s="91">
         <f t="shared" si="10"/>
         <v>1056.7</v>
       </c>
-      <c r="K43" s="44">
+      <c r="K43" s="91">
         <f t="shared" si="10"/>
         <v>30</v>
       </c>
-      <c r="L43" s="44">
+      <c r="L43" s="91">
         <f t="shared" si="10"/>
         <v>160</v>
       </c>
-      <c r="M43" s="44">
+      <c r="M43" s="91">
         <f t="shared" si="10"/>
         <v>145</v>
       </c>
-      <c r="N43" s="44">
+      <c r="N43" s="91">
         <f t="shared" si="10"/>
         <v>15</v>
       </c>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="44"/>
-      <c r="S43" s="44"/>
-      <c r="T43" s="44"/>
-      <c r="U43" s="44">
+      <c r="O43" s="91"/>
+      <c r="P43" s="91"/>
+      <c r="Q43" s="91"/>
+      <c r="R43" s="91"/>
+      <c r="S43" s="91"/>
+      <c r="T43" s="91"/>
+      <c r="U43" s="91">
         <f t="shared" si="10"/>
         <v>17.284739999999999</v>
       </c>
-      <c r="V43" s="44">
+      <c r="V43" s="91">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="W43" s="44">
+      <c r="W43" s="91">
         <f t="shared" si="10"/>
         <v>345.03</v>
       </c>
+      <c r="X43" s="89"/>
+      <c r="Y43" s="89"/>
+      <c r="Z43" s="89"/>
+      <c r="AA43" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>